<commit_message>
Added a new hard constraint matcher in PuLP
The PuLP version of hard constraints appears to be faster in some basic tests. (2.5 seconds vs 6.5 seconds)
</commit_message>
<xml_diff>
--- a/data/MOCK_Courses.xlsx
+++ b/data/MOCK_Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saahi\Documents (PC)\GitHub Repos\TAS_Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2D5DE6-4875-40CA-B92A-A170EBEC84B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE837185-07AA-4C80-956D-7DE0FBE84B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{11F8FF87-C9F4-408E-88A0-50D479BDF28C}"/>
   </bookViews>
@@ -556,7 +556,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2027,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05EA6C0-1409-48DC-89B2-CA1790DEA310}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J37"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2098,12 +2098,12 @@
         <v>80</v>
       </c>
       <c r="D2">
-        <f>FLOOR(B2/25, 1)</f>
-        <v>0</v>
+        <f>CEILING(B2/25, 1)</f>
+        <v>1</v>
       </c>
       <c r="E2">
-        <f>FLOOR(B2/30, 1)</f>
-        <v>0</v>
+        <f t="shared" ref="E2:E37" si="0">CEILING(B2/30, 1)</f>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
         <f>C2/15</f>
@@ -2114,12 +2114,12 @@
         <v>4.7058823529411766</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H37" si="0">C2/20</f>
+        <f t="shared" ref="H2:H37" si="1">C2/20</f>
         <v>4</v>
       </c>
       <c r="I2" s="1">
-        <f>FLOOR(C2/25, 1)</f>
-        <v>3</v>
+        <f t="shared" ref="I2:I37" si="2">CEILING(C2/25, 1)</f>
+        <v>4</v>
       </c>
       <c r="J2">
         <v>10</v>
@@ -2131,7 +2131,7 @@
         <v>400</v>
       </c>
       <c r="M2">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -2145,28 +2145,28 @@
         <v>80</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D37" si="1">FLOOR(B3/25, 1)</f>
-        <v>0</v>
+        <f t="shared" ref="D3:D37" si="3">CEILING(B3/25, 1)</f>
+        <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E37" si="2">FLOOR(B3/30, 1)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F37" si="3">C3/15</f>
+        <f t="shared" ref="F3:F37" si="4">C3/15</f>
         <v>5.333333333333333</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G37" si="4">C3/17</f>
+        <f t="shared" ref="G3:G37" si="5">C3/17</f>
         <v>4.7058823529411766</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I37" si="5">FLOOR(C3/25, 1)</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="J3">
         <v>6</v>
@@ -2178,7 +2178,7 @@
         <v>400</v>
       </c>
       <c r="M3">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -2192,28 +2192,28 @@
         <v>80</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.333333333333333</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.7058823529411766</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="J4">
         <v>11</v>
@@ -2225,7 +2225,7 @@
         <v>400</v>
       </c>
       <c r="M4">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2239,27 +2239,27 @@
         <v>350</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J5">
@@ -2272,7 +2272,7 @@
         <v>400</v>
       </c>
       <c r="M5">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -2286,27 +2286,27 @@
         <v>350</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J6">
@@ -2319,7 +2319,7 @@
         <v>400</v>
       </c>
       <c r="M6">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -2333,27 +2333,27 @@
         <v>350</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J7">
@@ -2366,7 +2366,7 @@
         <v>400</v>
       </c>
       <c r="M7">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -2380,27 +2380,27 @@
         <v>350</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J8">
@@ -2413,7 +2413,7 @@
         <v>400</v>
       </c>
       <c r="M8">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -2427,27 +2427,27 @@
         <v>350</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J9">
@@ -2460,7 +2460,7 @@
         <v>400</v>
       </c>
       <c r="M9">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -2474,27 +2474,27 @@
         <v>300</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J10">
@@ -2507,7 +2507,7 @@
         <v>400</v>
       </c>
       <c r="M10">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -2521,27 +2521,27 @@
         <v>300</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J11">
@@ -2554,7 +2554,7 @@
         <v>400</v>
       </c>
       <c r="M11">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -2568,27 +2568,27 @@
         <v>400</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.666666666666668</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.529411764705884</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J12">
@@ -2601,7 +2601,7 @@
         <v>400</v>
       </c>
       <c r="M12">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2615,27 +2615,27 @@
         <v>300</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J13">
@@ -2648,7 +2648,7 @@
         <v>400</v>
       </c>
       <c r="M13">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -2662,27 +2662,27 @@
         <v>300</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J14">
@@ -2695,7 +2695,7 @@
         <v>400</v>
       </c>
       <c r="M14">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -2709,27 +2709,27 @@
         <v>300</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J15">
@@ -2742,7 +2742,7 @@
         <v>400</v>
       </c>
       <c r="M15">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2756,27 +2756,27 @@
         <v>300</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J16">
@@ -2789,7 +2789,7 @@
         <v>400</v>
       </c>
       <c r="M16">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2803,27 +2803,27 @@
         <v>300</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J17">
@@ -2836,7 +2836,7 @@
         <v>400</v>
       </c>
       <c r="M17">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2850,27 +2850,27 @@
         <v>400</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.666666666666668</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.529411764705884</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J18">
@@ -2883,7 +2883,7 @@
         <v>400</v>
       </c>
       <c r="M18">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2897,27 +2897,27 @@
         <v>300</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J19">
@@ -2930,7 +2930,7 @@
         <v>400</v>
       </c>
       <c r="M19">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2944,27 +2944,27 @@
         <v>400</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.666666666666668</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.529411764705884</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J20">
@@ -2977,7 +2977,7 @@
         <v>400</v>
       </c>
       <c r="M20">
-        <v>300</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -2991,27 +2991,27 @@
         <v>300</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J21">
@@ -3023,8 +3023,8 @@
       <c r="L21">
         <v>400</v>
       </c>
-      <c r="M21" s="1">
-        <v>0</v>
+      <c r="M21">
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -3038,27 +3038,27 @@
         <v>200</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
       <c r="F22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.333333333333334</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.764705882352942</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="J22">
@@ -3070,8 +3070,8 @@
       <c r="L22">
         <v>400</v>
       </c>
-      <c r="M22" s="1">
-        <v>0</v>
+      <c r="M22">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -3085,27 +3085,27 @@
         <v>200</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
       <c r="F23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.333333333333334</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.764705882352942</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="J23">
@@ -3117,8 +3117,8 @@
       <c r="L23">
         <v>400</v>
       </c>
-      <c r="M23" s="1">
-        <v>0</v>
+      <c r="M23">
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -3132,27 +3132,27 @@
         <v>200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
       <c r="F24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.333333333333334</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11.764705882352942</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="J24">
@@ -3165,7 +3165,7 @@
         <v>400</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -3179,27 +3179,27 @@
         <v>400</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.666666666666668</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.529411764705884</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J25">
@@ -3212,7 +3212,7 @@
         <v>400</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -3226,27 +3226,27 @@
         <v>300</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="E26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J26">
@@ -3259,7 +3259,7 @@
         <v>400</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -3273,27 +3273,27 @@
         <v>150</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
       <c r="E27">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.8235294117647065</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J27">
@@ -3306,7 +3306,7 @@
         <v>400</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -3320,27 +3320,27 @@
         <v>300</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E28">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J28">
@@ -3353,7 +3353,7 @@
         <v>400</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -3367,27 +3367,27 @@
         <v>300</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E29">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.647058823529413</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J29">
@@ -3400,7 +3400,7 @@
         <v>400</v>
       </c>
       <c r="M29">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -3414,27 +3414,27 @@
         <v>100</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="E30">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666666666666667</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.882352941176471</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J30">
@@ -3447,7 +3447,7 @@
         <v>400</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -3461,27 +3461,27 @@
         <v>100</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="E31">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.666666666666667</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.882352941176471</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J31">
@@ -3494,7 +3494,7 @@
         <v>400</v>
       </c>
       <c r="M31">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -3508,27 +3508,27 @@
         <v>250</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E32">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.666666666666668</v>
       </c>
       <c r="G32" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.705882352941176</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="J32">
@@ -3541,7 +3541,7 @@
         <v>400</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -3555,27 +3555,27 @@
         <v>250</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E33">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.666666666666668</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.705882352941176</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="J33">
@@ -3588,7 +3588,7 @@
         <v>400</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -3602,27 +3602,27 @@
         <v>350</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E34">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J34">
@@ -3635,7 +3635,7 @@
         <v>400</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -3649,27 +3649,27 @@
         <v>350</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E35">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G35" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J35">
@@ -3682,7 +3682,7 @@
         <v>400</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -3696,27 +3696,27 @@
         <v>350</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E36">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G36" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J36">
@@ -3729,7 +3729,7 @@
         <v>400</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -3743,27 +3743,27 @@
         <v>350</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E37">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="G37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.588235294117649</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J37">
@@ -3776,7 +3776,7 @@
         <v>400</v>
       </c>
       <c r="M37">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
New Soft Constraint matcher and Output to CSV
</commit_message>
<xml_diff>
--- a/data/MOCK_Courses.xlsx
+++ b/data/MOCK_Courses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saahi\Documents (PC)\GitHub Repos\TAS_Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE837185-07AA-4C80-956D-7DE0FBE84B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E061AE4D-2DB4-4811-B786-00F9B41A62D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{11F8FF87-C9F4-408E-88A0-50D479BDF28C}"/>
   </bookViews>
@@ -2027,9 +2027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05EA6C0-1409-48DC-89B2-CA1790DEA310}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2130,8 +2128,8 @@
       <c r="L2">
         <v>400</v>
       </c>
-      <c r="M2">
-        <v>11</v>
+      <c r="M2" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -2177,8 +2175,8 @@
       <c r="L3">
         <v>400</v>
       </c>
-      <c r="M3">
-        <v>11</v>
+      <c r="M3" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -2224,8 +2222,8 @@
       <c r="L4">
         <v>400</v>
       </c>
-      <c r="M4">
-        <v>11</v>
+      <c r="M4" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2271,8 +2269,8 @@
       <c r="L5">
         <v>400</v>
       </c>
-      <c r="M5">
-        <v>11</v>
+      <c r="M5" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -2318,8 +2316,8 @@
       <c r="L6">
         <v>400</v>
       </c>
-      <c r="M6">
-        <v>11</v>
+      <c r="M6" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -2365,8 +2363,8 @@
       <c r="L7">
         <v>400</v>
       </c>
-      <c r="M7">
-        <v>11</v>
+      <c r="M7" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -2412,8 +2410,8 @@
       <c r="L8">
         <v>400</v>
       </c>
-      <c r="M8">
-        <v>11</v>
+      <c r="M8" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -2459,8 +2457,8 @@
       <c r="L9">
         <v>400</v>
       </c>
-      <c r="M9">
-        <v>11</v>
+      <c r="M9" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -2506,8 +2504,8 @@
       <c r="L10">
         <v>400</v>
       </c>
-      <c r="M10">
-        <v>11</v>
+      <c r="M10" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -2553,8 +2551,8 @@
       <c r="L11">
         <v>400</v>
       </c>
-      <c r="M11">
-        <v>11</v>
+      <c r="M11" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -2600,8 +2598,8 @@
       <c r="L12">
         <v>400</v>
       </c>
-      <c r="M12">
-        <v>11</v>
+      <c r="M12" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2647,8 +2645,8 @@
       <c r="L13">
         <v>400</v>
       </c>
-      <c r="M13">
-        <v>11</v>
+      <c r="M13" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -2695,7 +2693,7 @@
         <v>400</v>
       </c>
       <c r="M14">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -2742,7 +2740,7 @@
         <v>400</v>
       </c>
       <c r="M15">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2789,7 +2787,7 @@
         <v>400</v>
       </c>
       <c r="M16">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -2836,7 +2834,7 @@
         <v>400</v>
       </c>
       <c r="M17">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -2883,7 +2881,7 @@
         <v>400</v>
       </c>
       <c r="M18">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -2930,7 +2928,7 @@
         <v>400</v>
       </c>
       <c r="M19">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -2977,7 +2975,7 @@
         <v>400</v>
       </c>
       <c r="M20">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -3024,7 +3022,7 @@
         <v>400</v>
       </c>
       <c r="M21">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -3071,7 +3069,7 @@
         <v>400</v>
       </c>
       <c r="M22">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -3118,7 +3116,7 @@
         <v>400</v>
       </c>
       <c r="M23">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -3165,7 +3163,7 @@
         <v>400</v>
       </c>
       <c r="M24">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -3212,7 +3210,7 @@
         <v>400</v>
       </c>
       <c r="M25">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -3259,7 +3257,7 @@
         <v>400</v>
       </c>
       <c r="M26">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -3306,7 +3304,7 @@
         <v>400</v>
       </c>
       <c r="M27">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -3353,7 +3351,7 @@
         <v>400</v>
       </c>
       <c r="M28">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -3400,7 +3398,7 @@
         <v>400</v>
       </c>
       <c r="M29">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -3447,7 +3445,7 @@
         <v>400</v>
       </c>
       <c r="M30">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -3494,7 +3492,7 @@
         <v>400</v>
       </c>
       <c r="M31">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -3541,7 +3539,7 @@
         <v>400</v>
       </c>
       <c r="M32">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -3588,7 +3586,7 @@
         <v>400</v>
       </c>
       <c r="M33">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -3635,7 +3633,7 @@
         <v>400</v>
       </c>
       <c r="M34">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -3682,7 +3680,7 @@
         <v>400</v>
       </c>
       <c r="M35">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -3729,7 +3727,7 @@
         <v>400</v>
       </c>
       <c r="M36">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -3776,7 +3774,7 @@
         <v>400</v>
       </c>
       <c r="M37">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>